<commit_message>
few changes in test cases
</commit_message>
<xml_diff>
--- a/Excel/spiceJet.xlsx
+++ b/Excel/spiceJet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="16785" windowHeight="4140" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="16470" windowHeight="4125" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="signInwithMobile" sheetId="1" r:id="rId1"/>
@@ -12,13 +12,14 @@
     <sheet name="SignUpPage" sheetId="3" r:id="rId3"/>
     <sheet name="oneWayTrip" sheetId="4" r:id="rId4"/>
     <sheet name="roundTrip" sheetId="5" r:id="rId5"/>
+    <sheet name="signInwithNumber" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="25">
   <si>
     <t>SpiceJeat@1234</t>
   </si>
@@ -90,6 +91,9 @@
   </si>
   <si>
     <t>Kadapa</t>
+  </si>
+  <si>
+    <t>123456</t>
   </si>
 </sst>
 </file>
@@ -136,11 +140,12 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -513,7 +518,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -597,102 +602,92 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
     <col min="2" max="2" width="14.85546875" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" customWidth="1"/>
-    <col min="4" max="4" width="22" customWidth="1"/>
-    <col min="5" max="5" width="44.5703125" customWidth="1"/>
-    <col min="6" max="6" width="16.7109375" customWidth="1"/>
-    <col min="7" max="7" width="14.42578125" customWidth="1"/>
+    <col min="3" max="3" width="22" customWidth="1"/>
+    <col min="4" max="4" width="44.5703125" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>11</v>
       </c>
       <c r="B1" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="3">
-        <v>34630</v>
-      </c>
-      <c r="D1">
+      <c r="C1">
         <v>8522098804</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="E1" s="1" t="s">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>11</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="3">
-        <v>34476</v>
-      </c>
-      <c r="D2">
+      <c r="C2">
         <v>0</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F2" t="s">
+      <c r="E2" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>16</v>
       </c>
       <c r="B3" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="3">
-        <v>34478</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="C3" t="s">
         <v>17</v>
       </c>
+      <c r="D3" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="E3" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G3" s="1" t="s">
         <v>20</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E1" r:id="rId1"/>
-    <hyperlink ref="F1" r:id="rId2"/>
-    <hyperlink ref="G1" r:id="rId3"/>
-    <hyperlink ref="E2" r:id="rId4"/>
-    <hyperlink ref="G2" r:id="rId5"/>
-    <hyperlink ref="E3" r:id="rId6"/>
-    <hyperlink ref="F3" r:id="rId7"/>
-    <hyperlink ref="G3" r:id="rId8"/>
+    <hyperlink ref="D1" r:id="rId1"/>
+    <hyperlink ref="E1" r:id="rId2"/>
+    <hyperlink ref="F1" r:id="rId3"/>
+    <hyperlink ref="D2" r:id="rId4"/>
+    <hyperlink ref="F2" r:id="rId5"/>
+    <hyperlink ref="D3" r:id="rId6"/>
+    <hyperlink ref="E3" r:id="rId7"/>
+    <hyperlink ref="F3" r:id="rId8"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -745,7 +740,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -782,4 +777,50 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="39.85546875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="28" style="3" customWidth="1"/>
+    <col min="3" max="3" width="25.140625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="23.5703125" style="3" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="3">
+        <v>9989141338</v>
+      </c>
+      <c r="B1" s="3">
+        <v>1234556</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="3">
+        <v>9989141338</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>